<commit_message>
:ambulance: Hotfix for excel fortune
</commit_message>
<xml_diff>
--- a/static/fortune.xlsx
+++ b/static/fortune.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimth\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieun/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3BA030-C42F-48D0-95C3-7CB2E051201E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A8C93-9004-864A-A9CF-467DDD135C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10344" yWindow="684" windowWidth="28296" windowHeight="16164" xr2:uid="{8C0BFCB8-0E1C-0348-98DC-14521F4FF300}"/>
+    <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16060" xr2:uid="{8C0BFCB8-0E1C-0348-98DC-14521F4FF300}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>조금만 더 노력한다면 이번엔 A받을 것 같아요. 화이팅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>다음달의 큰 소비를 위해 이번 달은 절약을 해야 할 것 같아요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -111,26 +107,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>당신은 웃는 얼굴이 참 예뻐요. 당신의 미소가 힘이 돼요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>할 수 있다고 믿어 봐요. 생각보다 별 것 아닐 수도 있어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내일의 나는 오늘의 나보다 나을 거에요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>당신이 믿는 신념은 틀리지 않을 거에요. 이루미도 그것을 믿어요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1년전 당신을 떠올려 보세요. 분명 계속 성장했어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>오늘 하루는 무엇이든 긍정적으로 생각하는 노력을 해보세요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -160,6 +140,26 @@
   </si>
   <si>
     <t>한 번 뿐인 인생인데 무엇을 망설이나요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조금만 더 노력한다면 이번엔 좋은 점수 받을 것 같아요. 화이팅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일 년 전 당신을 떠올려 보세요. 분명 계속 성장했어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내일의 나는 오늘의 나보다 나을 거에요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할 수 있다고 믿어 봐요. 생각보다 별 것 아닐 수도 있어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 웃는 얼굴이 참 예뻐요. 당신의 미소가 힘이 돼요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -167,7 +167,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -526,183 +526,183 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABB5A00-D612-C746-BD12-7B45F12E94F3}">
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="73.7265625" customWidth="1"/>
+    <col min="1" max="1" width="73.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:memo: Update excel with /r/n
</commit_message>
<xml_diff>
--- a/static/fortune.xlsx
+++ b/static/fortune.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieun/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A8C93-9004-864A-A9CF-467DDD135C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E2DEF7-47B1-1444-B71B-2080DA4F3C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16060" xr2:uid="{8C0BFCB8-0E1C-0348-98DC-14521F4FF300}"/>
   </bookViews>
@@ -31,135 +31,135 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>오늘은 예상치 못한 나의 언행으로 위험해질 수 있을 것 같아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화나 연극을 보세요. 생각지 못한 영감을 얻을 것 같아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>노력은 배신하지 않아요. 성실한 당신을 이루미는 믿어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>책임감이 부담이 될 수 있지만 주변은 당신에게 의지해요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>무엇보다도 나 자신을 사랑하는 것이 중요해요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>행복은 거창한 것이 아니라 작은 것에서 시작해요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 가위바위보를 해야 한다면 주먹을 내보는 건 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혹시 연락을 망설이고 있다면 오늘이 그 기회일 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미안하다는 말을 먼저 해보는 건 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새로운 인연이 마음에 든다면 적극적으로 다가가 보세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다음달의 큰 소비를 위해 이번 달은 절약을 해야 할 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지금 고민 하고 있는 일이 있다면 하는 것이 좋을 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감정을 숨기지 마세요. 상대는 당신의 진심을 기다리고 있어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지금 하고 싶은 일이 있군요. 망설이지 마세요 잘 될 거에요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 행운의 색은 푸른색입니다. 시원시원한 모습을 보여주세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작은 말이라도 칭찬해보세요. 고래가 춤을 출지도 모르니까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신은 반전매력은 솔직한 모습을 보여줄 때 느껴져요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>너무 과한 계획을 세우지는 않았나요. 재정비를 해보세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당분간 지켜보는 것이 좋을 것 같아요. 타이밍이 중요해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신이 믿는 신념은 틀리지 않을 거에요. 이루미도 그것을 믿어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 하루는 무엇이든 긍정적으로 생각하는 노력을 해보세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기분 전환하러 이번 방학엔 여행을 떠나보는 것은 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오지 않은 미래를 걱정하는 것 보다 마주한 현재에 최선을 다하세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 것은 나의 태도에 달려있어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리는 아직 우리가 보석인지 몰라요. 당신은 특별해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>익숙함에 속아 소중함을 잃지 말자구요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘은 부모님께 전화 한 통 드리는 것이 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한 번 뿐인 인생인데 무엇을 망설이나요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조금만 더 노력한다면 이번엔 좋은 점수 받을 것 같아요. 화이팅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일 년 전 당신을 떠올려 보세요. 분명 계속 성장했어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내일의 나는 오늘의 나보다 나을 거에요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>할 수 있다고 믿어 봐요. 생각보다 별 것 아닐 수도 있어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신은 웃는 얼굴이 참 예뻐요. 당신의 미소가 힘이 돼요.</t>
+    <t>오늘 가위바위보를 해야 한다면\r\n주먹을 내보는 건 어떨까요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시 연락을 망설이고 있다면\r\n오늘이 그 기회일 것 같아요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미안하다는 말을\r\n먼저 해보는 건 어떨까요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 인연이 마음에 든다면\r\n적극적으로 다가가 보세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조금만 더 노력한다면\r\n이번엔 좋은 점수 받을 거예요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음달의 큰 소비를 위해\r\n이번 달은 절약을 해야 할 것 같아요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금 고민 하고 있는 일이 있다면\r\n하는 것이 좋을 것 같아요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감정을 숨기지 마세요.\r\n상대는 당신의 진심을 기다리고 있어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금 하고 싶은 일이 있군요.\r\n망설이지 마세요 잘 될 거에요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘 행운의 색은 푸른색입니다.\r\n시원시원한 모습을 보여주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은 말이라도 칭찬해보세요.\r\n고래가 춤을 출지도 모르니까요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 반전매력은\r\n솔직한 모습을 보여줄 때 느껴져요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너무 과한 계획을 세우지는 않았나요.\r\n재정비를 해보세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은 예상치 못한 나의 언행으로\r\n위험해질 수 있을 것 같아요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화나 연극을 보세요.\r\n생각지 못한 영감을 얻을 것 같아요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당분간 지켜보는 것이 좋을 것 같아요.\r\n타이밍이 중요해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노력은 배신하지 않아요.\r\n성실한 당신을 이루미는 믿어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책임감이 부담이 될 수 있지만\r\n주변은 당신에게 의지해요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 웃는 얼굴이 참 예뻐요.\r\n당신의 미소가 힘이 돼요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할 수 있다고 믿어 봐요.\r\n생각보다 별 것 아닐 수도 있어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내일의 나는\r\n오늘의 나보다 나을 거에요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신이 믿는 신념은 틀리지 않을 거에요.\r\n이루미도 그것을 믿어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일 년 전 당신을 떠올려 보세요.\r\n분명 계속 성장했어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무엇보다도 나 자신을\r\n사랑하는 것이 중요해요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행복은 거창한 것이 아니라\r\n작은 것에서 시작해요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오지 않은 미래를 걱정하는 것보다\r\n마주한 현재에 최선을 다하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기분 전환하러 이번 방학엔\r\n여행을 떠나보는 것은 어떨까요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘 하루는 무엇이든\r\n긍정적으로 생각하는 노력을 해보세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 것은 나의 태도에 달려있어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리는 아직 우리가 보석인지 몰라요.\r\n당신은 특별해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>익숙함에 속아 소중함을 잃지 말자구요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 번 뿐인 인생인데 무엇을 망설이나요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은 부모님께 전화 한 통\r\n드리는 것이 어떨까요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -527,7 +527,7 @@
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -542,167 +542,167 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:pencil2: Fixed excel typos
</commit_message>
<xml_diff>
--- a/static/fortune.xlsx
+++ b/static/fortune.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieun/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE42631-DC2A-8B43-A2ED-551A4F811C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA12E23-D535-CB49-9C1F-952872A347DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16060" xr2:uid="{8C0BFCB8-0E1C-0348-98DC-14521F4FF300}"/>
   </bookViews>
@@ -59,66 +59,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>감정을 숨기지 마세요.\r\n상대는 당신의 진심을 기다리고 있어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지금 하고 싶은 일이 있군요.\r\n망설이지 마세요 잘 될 거에요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 행운의 색은 푸른색입니다.\r\n시원시원한 모습을 보여주세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작은 말이라도 칭찬해보세요.\r\n고래가 춤을 출지도 모르니까요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>너무 과한 계획을 세우지는 않았나요.\r\n재정비를 해보세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>오늘은 예상치 못한 나의 언행으로\r\n위험해질 수 있을 것 같아요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화나 연극을 보세요.\r\n생각지 못한 영감을 얻을 것 같아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당분간 지켜보는 것이 좋을 것 같아요.\r\n타이밍이 중요해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>노력은 배신하지 않아요.\r\n성실한 당신을 이루미는 믿어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>책임감이 부담이 될 수 있지만\r\n주변은 당신에게 의지해요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>당신은 웃는 얼굴이 참 예뻐요.\r\n당신의 미소가 힘이 돼요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>할 수 있다고 믿어 봐요.\r\n생각보다 별 것 아닐 수도 있어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>내일의 나는\r\n오늘의 나보다 나을 거에요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>당신이 믿는 신념은 틀리지 않을 거에요.\r\n이루미도 그것을 믿어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일 년 전 당신을 떠올려 보세요.\r\n분명 계속 성장했어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>무엇보다도 나 자신을\r\n사랑하는 것이 중요해요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>우리는 아직 우리가 보석인지 몰라요.\r\n당신은 특별해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>익숙함에 속아 소중함을 잃지 말자구요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -160,6 +108,58 @@
   </si>
   <si>
     <t>당신의 반전매력은\r\n솔직한 모습을 보여줄 때 느껴져요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신이 믿는 신념은 틀리지 않을 거에요. 이루미도 그것을 믿어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감정을 숨기지 마세요. \r\n상대는 당신의 진심을 기다리고 있어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금 하고 싶은 일이 있군요. \r\n망설이지 마세요 잘 될 거에요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘 행운의 색은 푸른색입니다. \r\n시원시원한 모습을 보여주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은 말이라도 칭찬해보세요. \r\n고래가 춤을 출지도 모르니까요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너무 과한 계획을 세우지는 않았나요. \r\n재정비를 해보세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화나 연극을 보세요. \r\n생각지 못한 영감을 얻을 것 같아요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당분간 지켜보는 것이 좋을 것 같아요. \r\n타이밍이 중요해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노력은 배신하지 않아요. \r\n성실한 당신을 이루미는 믿어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 웃는 얼굴이 참 예뻐요. \r\n당신의 미소가 힘이 돼요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할 수 있다고 믿어 봐요. \r\n생각보다 별 것 아닐 수도 있어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일 년 전 당신을 떠올려 보세요. \r\n분명 계속 성장했어요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리는 아직 우리가 보석인지 몰라요. \r\n당신은 특별해요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -527,7 +527,7 @@
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -577,72 +577,72 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:1">
@@ -652,57 +652,57 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:pencil2: Fix typos in excel
</commit_message>
<xml_diff>
--- a/static/fortune.xlsx
+++ b/static/fortune.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieun/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA12E23-D535-CB49-9C1F-952872A347DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDC0118-2C4E-4546-9223-3DADF48EEB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16060" xr2:uid="{8C0BFCB8-0E1C-0348-98DC-14521F4FF300}"/>
   </bookViews>
@@ -47,119 +47,119 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>조금만 더 노력한다면\r\n이번엔 좋은 점수 받을 거예요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다음달의 큰 소비를 위해\r\n이번 달은 절약을 해야 할 것 같아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지금 고민 하고 있는 일이 있다면\r\n하는 것이 좋을 것 같아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘은 예상치 못한 나의 언행으로\r\n위험해질 수 있을 것 같아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>책임감이 부담이 될 수 있지만\r\n주변은 당신에게 의지해요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내일의 나는\r\n오늘의 나보다 나을 거에요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>무엇보다도 나 자신을\r\n사랑하는 것이 중요해요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>행복은 거창한 것이 아니라\r\n작은 것에서 시작해요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오지 않은 미래를 걱정하는 것보다\r\n마주한 현재에 최선을 다하세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기분 전환하러 이번 방학엔\r\n여행을 떠나보는 것은 어떨까요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 하루는 무엇이든\r\n긍정적으로 생각하는 노력을 해보세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 것은 나의 태도에 달려있어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>익숙함에 속아 소중함을 잃지 말자구요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한 번 뿐인 인생인데 무엇을 망설이나요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘은 부모님께 전화 한 통\r\n드리는 것이 어떨까요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신의 반전매력은\r\n솔직한 모습을 보여줄 때 느껴져요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신이 믿는 신념은 틀리지 않을 거에요. 이루미도 그것을 믿어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감정을 숨기지 마세요. \r\n상대는 당신의 진심을 기다리고 있어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지금 하고 싶은 일이 있군요. \r\n망설이지 마세요 잘 될 거에요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 행운의 색은 푸른색입니다. \r\n시원시원한 모습을 보여주세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작은 말이라도 칭찬해보세요. \r\n고래가 춤을 출지도 모르니까요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>너무 과한 계획을 세우지는 않았나요. \r\n재정비를 해보세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화나 연극을 보세요. \r\n생각지 못한 영감을 얻을 것 같아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당분간 지켜보는 것이 좋을 것 같아요. \r\n타이밍이 중요해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>노력은 배신하지 않아요. \r\n성실한 당신을 이루미는 믿어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신은 웃는 얼굴이 참 예뻐요. \r\n당신의 미소가 힘이 돼요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>할 수 있다고 믿어 봐요. \r\n생각보다 별 것 아닐 수도 있어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일 년 전 당신을 떠올려 보세요. \r\n분명 계속 성장했어요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리는 아직 우리가 보석인지 몰라요. \r\n당신은 특별해요</t>
+    <t>조금만 더 노력한다면\r\n이번엔 좋은 점수 받을 거예요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음달의 큰 소비를 위해\r\n이번 달은 절약을 해야 할 것 같아요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금 고민 하고 있는 일이 있다면\r\n하는 것이 좋을 것 같아요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신의 반전매력은\r\n솔직한 모습을 보여줄 때 느껴져요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은 예상치 못한 나의 언행으로\r\n위험해질 수 있을 것 같아요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감정을 숨기지 마세요\r\n상대는 당신의 진심을 기다리고 있어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금 하고 싶은 일이 있군요\r\n망설이지 마세요 잘 될 거에요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘 행운의 색은 푸른색입니다\r\n시원시원한 모습을 보여주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은 말이라도 칭찬해보세요\r\n고래가 춤을 출지도 모르니까요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너무 과한 계획을 세우지는 않았나요\r\n재정비를 해보세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화나 연극을 보세요\r\n생각지 못한 영감을 얻을 것 같아요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당분간 지켜보는 것이 좋을 것 같아요\r\n타이밍이 중요해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노력은 배신하지 않아요\r\n성실한 당신을 이루미는 믿어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책임감이 부담이 될 수 있지만\r\n주변은 당신에게 의지해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 웃는 얼굴이 참 예뻐요\r\n당신의 미소가 힘이 돼요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할 수 있다고 믿어 봐요\r\n생각보다 별 것 아닐 수도 있어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내일의 나는\r\n오늘의 나보다 나을 거에요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신이 믿는 신념은 틀리지 않을 거에요 이루미도 그것을 믿어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일 년 전 당신을 떠올려 보세요\r\n분명 계속 성장했어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘 하루는 무엇이든\r\n긍정적으로 생각하는 노력을 해보세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무엇보다도 나 자신을\r\n사랑하는 것이 중요해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행복은 거창한 것이 아니라\r\n작은 것에서 시작해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기분 전환하러 이번 방학엔\r\n여행을 떠나보는 것은 어떨까요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오지 않은 미래를 걱정하는 것보다\r\n마주한 현재에 최선을 다하세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 것은 나의 태도에 달려있어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리는 아직 우리가 보석인지 몰라요\r\n당신은 특별해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>익숙함에 속아 소중함을 잃지 말자구요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은 부모님께 전화 한 통\r\n드리는 것이 어떨까요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 번 뿐인 인생인데 무엇을 망설이나요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -527,7 +527,7 @@
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -577,132 +577,132 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:memo: Update fortune document
</commit_message>
<xml_diff>
--- a/static/fortune.xlsx
+++ b/static/fortune.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieun/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDC0118-2C4E-4546-9223-3DADF48EEB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ED77734-F9D3-7B45-B0B7-6D39FF8B0279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16060" xr2:uid="{8C0BFCB8-0E1C-0348-98DC-14521F4FF300}"/>
   </bookViews>
@@ -25,141 +25,137 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>fortune</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>오늘 가위바위보를 해야 한다면\r\n주먹을 내보는 건 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혹시 연락을 망설이고 있다면\r\n오늘이 그 기회일 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미안하다는 말을\r\n먼저 해보는 건 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새로운 인연이 마음에 든다면\r\n적극적으로 다가가 보세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조금만 더 노력한다면\r\n이번엔 좋은 점수 받을 거예요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다음달의 큰 소비를 위해\r\n이번 달은 절약을 해야 할 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지금 고민 하고 있는 일이 있다면\r\n하는 것이 좋을 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신의 반전매력은\r\n솔직한 모습을 보여줄 때 느껴져요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘은 예상치 못한 나의 언행으로\r\n위험해질 수 있을 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감정을 숨기지 마세요\r\n상대는 당신의 진심을 기다리고 있어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지금 하고 싶은 일이 있군요\r\n망설이지 마세요 잘 될 거에요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 행운의 색은 푸른색입니다\r\n시원시원한 모습을 보여주세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작은 말이라도 칭찬해보세요\r\n고래가 춤을 출지도 모르니까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>너무 과한 계획을 세우지는 않았나요\r\n재정비를 해보세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화나 연극을 보세요\r\n생각지 못한 영감을 얻을 것 같아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당분간 지켜보는 것이 좋을 것 같아요\r\n타이밍이 중요해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>노력은 배신하지 않아요\r\n성실한 당신을 이루미는 믿어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>책임감이 부담이 될 수 있지만\r\n주변은 당신에게 의지해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신은 웃는 얼굴이 참 예뻐요\r\n당신의 미소가 힘이 돼요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>할 수 있다고 믿어 봐요\r\n생각보다 별 것 아닐 수도 있어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내일의 나는\r\n오늘의 나보다 나을 거에요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>당신이 믿는 신념은 틀리지 않을 거에요 이루미도 그것을 믿어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일 년 전 당신을 떠올려 보세요\r\n분명 계속 성장했어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 하루는 무엇이든\r\n긍정적으로 생각하는 노력을 해보세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>무엇보다도 나 자신을\r\n사랑하는 것이 중요해요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>행복은 거창한 것이 아니라\r\n작은 것에서 시작해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기분 전환하러 이번 방학엔\r\n여행을 떠나보는 것은 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오지 않은 미래를 걱정하는 것보다\r\n마주한 현재에 최선을 다하세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 것은 나의 태도에 달려있어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리는 아직 우리가 보석인지 몰라요\r\n당신은 특별해요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>익숙함에 속아 소중함을 잃지 말자구요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘은 부모님께 전화 한 통\r\n드리는 것이 어떨까요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한 번 뿐인 인생인데 무엇을 망설이나요</t>
+    <t>가위바위보를 한다면\r\n주먹을 내보는 건 어떨까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연락을 망설이고 있다면\r\n오늘이 기회일 것 같아요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진심어린 사과를\r\n먼저 해보면 어떨까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로 알게된 인연에게\r\n관심이 생긴다면\r\n적극적으로 다가가 보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미래를 위해 이번 달은\r\n절약을 해야 할 것 같아요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고민 하고 있다면\r\n한번 해보는 게 어때요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감정을 숨기지 마세요!\r\n당신을 기다리고 있어요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칭찬을 해보는 건 어떨까요?\r\n고래가 춤을 추길 바라면서요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>솔직한 모습을 보여줄 때\r\n당신의 매력은 더욱 커져요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금 지쳐있나요?\r\n재정비를 해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은 나의 언행을\r\n조심할 필요가 있어요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영감이 필요하다면\r\n영화를 보는 건 어떨까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>섣부른 결정은 피하세요!\r\n타이밍이 중요해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노력은 배신하지 않아요\r\n성실한 당신을 믿어주세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 큰 존재입니다!\r\n주변은 당신에게 의지해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웃는 얼굴이 제일 예뻐요\r\n당신의 미소가 힘이 돼요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너무 걱정 말아요\r\n별 것 아닐 거예요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조금만 더 노력한다면\r\n좋은 일이 생길 거예요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하고 싶은 일이 있군요?\r\n망설이지 마세요\r\n잘 될 거예요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내일의 나는\r\n오늘의 나보다 나을 거예요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신이 믿는 신념은\r\n틀리지 않을 거예요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼마 전을 떠올려 보세요\r\n분명 계속 성장했어요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘 하루는 무엇이든\r\n긍정적으로 생각해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행복은\r\n거창한 것이 아니라\r\n작은 것에서 시작해요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이번 방학엔\r\n나를 위한 여행을\r\n떠나보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 것은\r\n나의 태도에 달렸어요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리는 아직\r\n우리가 가치를 몰라요\r\n당신은 특별해요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>익숙함에 속아\r\n소중함을 잃지 말자구요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은 부모님께\r\n전화 한 통 드려보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 번 뿐인 인생\r\n무엇을 망설이나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오지 않은 미래를\r\n걱정하는 것보다\r\n마주한 현재에\r\n최선을 다해보세요!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -228,9 +224,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +264,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -374,7 +370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,7 +512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABB5A00-D612-C746-BD12-7B45F12E94F3}">
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -542,27 +538,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -577,87 +573,87 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:1">
@@ -672,37 +668,32 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:art: Change fortune files
</commit_message>
<xml_diff>
--- a/static/fortune.xlsx
+++ b/static/fortune.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieun/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ED77734-F9D3-7B45-B0B7-6D39FF8B0279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AC5A48-2E43-E849-985F-4DEB312313D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16060" xr2:uid="{8C0BFCB8-0E1C-0348-98DC-14521F4FF300}"/>
   </bookViews>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>고민 하고 있다면\r\n한번 해보는 게 어때요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>감정을 숨기지 마세요!\r\n당신을 기다리고 있어요!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,10 +135,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>우리는 아직\r\n우리가 가치를 몰라요\r\n당신은 특별해요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>익숙함에 속아\r\n소중함을 잃지 말자구요!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -156,6 +148,14 @@
   </si>
   <si>
     <t>오지 않은 미래를\r\n걱정하는 것보다\r\n마주한 현재에\r\n최선을 다해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리는 아직\r\n우리의 가치를 몰라요\r\n당신은 특별해요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고민하고 있다면\r\n한번 해보는 게 어때요?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -523,7 +523,7 @@
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -568,87 +568,87 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
@@ -658,42 +658,42 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>